<commit_message>
admin get user added
</commit_message>
<xml_diff>
--- a/apis.xlsx
+++ b/apis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IBA\Semestor 6\webdev\Thrift Store\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D52500-2132-4A2E-BDD8-6EB3139F0182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA73ACB8-B7C0-48D9-A633-5C1BD3ED59F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{F1FDD628-6884-4E21-B61A-2CE76824DB8F}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{F1FDD628-6884-4E21-B61A-2CE76824DB8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Buyer" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="90">
   <si>
     <t>API</t>
   </si>
@@ -279,9 +279,6 @@
     <t>getuser</t>
   </si>
   <si>
-    <t>token, firstname, lastname, username</t>
-  </si>
-  <si>
     <t>progress</t>
   </si>
   <si>
@@ -310,6 +307,9 @@
   </si>
   <si>
     <t>array&lt;orderdetail&gt;</t>
+  </si>
+  <si>
+    <t>tested</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -427,6 +427,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -747,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFA796C-7BC2-4338-AD3D-8C08A94134AD}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="144" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A9" zoomScale="144" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -770,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -782,7 +785,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -791,11 +794,11 @@
       <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>55</v>
@@ -841,7 +844,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>26</v>
@@ -861,19 +864,23 @@
       <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
@@ -944,7 +951,7 @@
       </c>
       <c r="D16" s="9"/>
     </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -964,12 +971,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>38</v>
@@ -1000,13 +1007,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="D23" s="8"/>
     </row>
@@ -1052,7 +1059,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1152,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{785618A5-B900-4482-A589-C8AADA4C14ED}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1184,7 +1191,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1221,6 +1228,20 @@
         <v>40</v>
       </c>
       <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1231,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A3B489-13FF-422D-A02A-B7A8117B432E}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="218" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1271,7 +1292,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update user altered and get profile made
</commit_message>
<xml_diff>
--- a/apis.xlsx
+++ b/apis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IBA\Semestor 6\webdev\Thrift Store\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA73ACB8-B7C0-48D9-A633-5C1BD3ED59F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423CD6C0-EA82-42A6-B2E1-22BE74274D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{F1FDD628-6884-4E21-B61A-2CE76824DB8F}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{F1FDD628-6884-4E21-B61A-2CE76824DB8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Buyer" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="95">
   <si>
     <t>API</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>create order</t>
-  </si>
-  <si>
-    <t>update profile</t>
   </si>
   <si>
     <t>API desc</t>
@@ -234,9 +231,6 @@
     <t>isrestricted:bool</t>
   </si>
   <si>
-    <t>add shipment</t>
-  </si>
-  <si>
     <t>delete shipment</t>
   </si>
   <si>
@@ -310,6 +304,27 @@
   </si>
   <si>
     <t>tested</t>
+  </si>
+  <si>
+    <t>getalluser</t>
+  </si>
+  <si>
+    <t>array&lt;users&gt;</t>
+  </si>
+  <si>
+    <t>delete user</t>
+  </si>
+  <si>
+    <t>token, username</t>
+  </si>
+  <si>
+    <t>getprofile</t>
+  </si>
+  <si>
+    <t>add shipper</t>
+  </si>
+  <si>
+    <t>update user</t>
   </si>
 </sst>
 </file>
@@ -750,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFA796C-7BC2-4338-AD3D-8C08A94134AD}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="144" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -773,7 +788,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -781,105 +796,105 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -887,10 +902,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" s="8"/>
     </row>
@@ -899,43 +914,43 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="8"/>
     </row>
@@ -944,76 +959,80 @@
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="9"/>
+        <v>34</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="D23" s="8"/>
     </row>
@@ -1027,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB005B9-1A29-49DE-85F5-CA65856DDA0B}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="144" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="144" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1047,108 +1066,96 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F1" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" ht="44.65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="F9" s="8"/>
     </row>
@@ -1159,22 +1166,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{785618A5-B900-4482-A589-C8AADA4C14ED}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="18.41796875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="8.83984375" style="1"/>
-    <col min="4" max="4" width="43" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.41796875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83984375" style="1"/>
+    <col min="2" max="2" width="43" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.41796875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1182,65 +1188,101 @@
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="44.65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>89</v>
+      <c r="C8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1264,35 +1306,35 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>